<commit_message>
Changes related to Qlik, Mail, CSV, and Util
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shailendra.rajawat\git\iotronApex5\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6FF674-4759-4960-8975-3AA94DB8B8B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961F7CFA-CCCB-4DE2-B3A8-A627BC191C0D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="12825" tabRatio="988" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="12825" tabRatio="988" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UAT" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1945" uniqueCount="684">
   <si>
     <t>url</t>
   </si>
@@ -1500,9 +1500,6 @@
     <t>SHAILENDRA.AUSOP.OR_T14</t>
   </si>
   <si>
-    <t>Spidey@1990</t>
-  </si>
-  <si>
     <t>SHAILENDRA.NGC.KPN_Op4_T01</t>
   </si>
   <si>
@@ -1608,9 +1605,6 @@
     <t>IOTRON_ADMIN,IOTRON What-If,MANAGER,ACCOUNT MANAGER,OPERATIONS SUPPORT 2</t>
   </si>
   <si>
-    <t>Auto$120219123312</t>
-  </si>
-  <si>
     <t>Auto$120219123340</t>
   </si>
   <si>
@@ -1800,9 +1794,6 @@
     <t>IOTRON_ADMIN,IOTRON What-If,IOTRON_SETT_BRIDGE_CRUD_USER,MANAGER,IOTRON_DT_Budget,IOTRON_DT_Flash,IOTRON_Deal_Tracker</t>
   </si>
   <si>
-    <t>Auto$040319195809</t>
-  </si>
-  <si>
     <t>micky</t>
   </si>
   <si>
@@ -1851,9 +1842,6 @@
     <t>DEV_SR</t>
   </si>
   <si>
-    <t>Nkj45jgsD8</t>
-  </si>
-  <si>
     <t>PREPROD</t>
   </si>
   <si>
@@ -2061,9 +2049,6 @@
     <t>Auto$170419115557</t>
   </si>
   <si>
-    <t>shailendra.rajawat@nextgenclearing.com,prafull.barve@nextgenclearing.com,ivana.jandrecic@nextgenclearing.com,dario.curjak@nextgenclearing.com</t>
-  </si>
-  <si>
     <t>micky.priya</t>
   </si>
   <si>
@@ -2074,6 +2059,48 @@
   </si>
   <si>
     <t>https://fch.nextgenclearing.com/pls/apex/f?p=10132:35:11449201093111::NO:::</t>
+  </si>
+  <si>
+    <t>prafull.barve@nextgenclearing.com</t>
+  </si>
+  <si>
+    <t>ivana.jandrecic@nextgenclearing.com</t>
+  </si>
+  <si>
+    <t>dario.curjak@nextgenclearing.com</t>
+  </si>
+  <si>
+    <t>aarjav.thakore@nextgenclearing.com</t>
+  </si>
+  <si>
+    <t>micky.priya@nextgenclearing.com</t>
+  </si>
+  <si>
+    <t>kelvin.egoh@nextgenclearing.com</t>
+  </si>
+  <si>
+    <t>vaibhav.aggarwal@nextgenclearing.com</t>
+  </si>
+  <si>
+    <t>IOTRON</t>
+  </si>
+  <si>
+    <t>QLIK</t>
+  </si>
+  <si>
+    <t>Individual Emails for formula &amp;","&amp;</t>
+  </si>
+  <si>
+    <t>Team Info just for Information, not used anywhere in framework</t>
+  </si>
+  <si>
+    <t>Auto$030519144918</t>
+  </si>
+  <si>
+    <t>Thanos@1990</t>
+  </si>
+  <si>
+    <t>WAPTRQ6851</t>
   </si>
 </sst>
 </file>
@@ -2241,7 +2268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2304,6 +2331,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6117,19 +6147,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B1" t="s">
+        <v>590</v>
+      </c>
+      <c r="C1" t="s">
+        <v>591</v>
+      </c>
+      <c r="D1" t="s">
         <v>592</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>593</v>
-      </c>
-      <c r="C1" t="s">
-        <v>594</v>
-      </c>
-      <c r="D1" t="s">
-        <v>595</v>
-      </c>
-      <c r="E1" t="s">
-        <v>596</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -6137,42 +6167,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="B2" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C2">
         <v>1521</v>
       </c>
       <c r="D2" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="E2" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>600</v>
+        <v>683</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B3" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C3">
         <v>1521</v>
       </c>
       <c r="D3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="E3" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -6184,8 +6214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK67"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6248,8 +6278,8 @@
       <c r="C2" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="D2" s="29" t="s">
-        <v>583</v>
+      <c r="D2" s="31" t="s">
+        <v>602</v>
       </c>
       <c r="E2" s="28" t="s">
         <v>51</v>
@@ -6278,10 +6308,10 @@
         <v>220</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F3" s="28" t="s">
         <v>52</v>
@@ -6296,7 +6326,7 @@
         <v>55</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="K3" s="28" t="s">
         <v>232</v>
@@ -6311,7 +6341,7 @@
         <v>221</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E4" s="28" t="s">
         <v>80</v>
@@ -6342,7 +6372,7 @@
         <v>33</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="E5" s="28" t="s">
         <v>32</v>
@@ -6373,7 +6403,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="E6" s="28" t="s">
         <v>34</v>
@@ -6404,7 +6434,7 @@
         <v>39</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="E7" s="28" t="s">
         <v>51</v>
@@ -6422,7 +6452,7 @@
         <v>55</v>
       </c>
       <c r="J7" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K7" s="28"/>
     </row>
@@ -6435,7 +6465,7 @@
         <v>227</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E8" s="28" t="s">
         <v>228</v>
@@ -6466,7 +6496,7 @@
         <v>230</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="E9" s="28" t="s">
         <v>231</v>
@@ -6499,7 +6529,7 @@
         <v>234</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="E10" s="28" t="s">
         <v>235</v>
@@ -6530,7 +6560,7 @@
         <v>240</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="E11" s="28" t="s">
         <v>241</v>
@@ -6563,7 +6593,7 @@
         <v>408</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="E12" s="28" t="s">
         <v>51</v>
@@ -6581,7 +6611,7 @@
         <v>55</v>
       </c>
       <c r="J12" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K12" s="28"/>
     </row>
@@ -6594,7 +6624,7 @@
         <v>479</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="E13" s="28" t="s">
         <v>34</v>
@@ -6625,7 +6655,7 @@
         <v>409</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="E14" s="28" t="s">
         <v>51</v>
@@ -6643,7 +6673,7 @@
         <v>55</v>
       </c>
       <c r="J14" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K14" s="28"/>
     </row>
@@ -6656,7 +6686,7 @@
         <v>480</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="E15" s="28" t="s">
         <v>34</v>
@@ -6690,7 +6720,7 @@
         <v>410</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="E16" s="28" t="s">
         <v>51</v>
@@ -6708,7 +6738,7 @@
         <v>55</v>
       </c>
       <c r="J16" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K16" s="28"/>
     </row>
@@ -6721,7 +6751,7 @@
         <v>411</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="E17" s="28" t="s">
         <v>51</v>
@@ -6739,7 +6769,7 @@
         <v>55</v>
       </c>
       <c r="J17" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K17" s="28"/>
     </row>
@@ -6752,7 +6782,7 @@
         <v>412</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="E18" s="28" t="s">
         <v>51</v>
@@ -6770,7 +6800,7 @@
         <v>55</v>
       </c>
       <c r="J18" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K18" s="28"/>
     </row>
@@ -6783,7 +6813,7 @@
         <v>413</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="E19" s="28" t="s">
         <v>51</v>
@@ -6801,7 +6831,7 @@
         <v>55</v>
       </c>
       <c r="J19" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K19" s="28"/>
     </row>
@@ -6814,7 +6844,7 @@
         <v>414</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="E20" s="28" t="s">
         <v>51</v>
@@ -6832,7 +6862,7 @@
         <v>55</v>
       </c>
       <c r="J20" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K20" s="28"/>
     </row>
@@ -6845,7 +6875,7 @@
         <v>481</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="E21" s="28" t="s">
         <v>34</v>
@@ -6876,7 +6906,7 @@
         <v>451</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="E22" s="28" t="s">
         <v>51</v>
@@ -6894,7 +6924,7 @@
         <v>55</v>
       </c>
       <c r="J22" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K22" s="28"/>
     </row>
@@ -6907,7 +6937,7 @@
         <v>482</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="E23" s="28" t="s">
         <v>34</v>
@@ -6938,7 +6968,7 @@
         <v>453</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="E24" s="28" t="s">
         <v>51</v>
@@ -6956,7 +6986,7 @@
         <v>55</v>
       </c>
       <c r="J24" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K24" s="28"/>
     </row>
@@ -6969,7 +6999,7 @@
         <v>415</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="E25" s="28" t="s">
         <v>51</v>
@@ -6987,7 +7017,7 @@
         <v>55</v>
       </c>
       <c r="J25" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K25" s="28"/>
     </row>
@@ -7000,7 +7030,7 @@
         <v>416</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="E26" s="28" t="s">
         <v>51</v>
@@ -7018,7 +7048,7 @@
         <v>55</v>
       </c>
       <c r="J26" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K26" s="28"/>
     </row>
@@ -7031,7 +7061,7 @@
         <v>431</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="E27" s="28" t="s">
         <v>51</v>
@@ -7049,7 +7079,7 @@
         <v>55</v>
       </c>
       <c r="J27" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K27" s="28"/>
     </row>
@@ -7062,7 +7092,7 @@
         <v>436</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="E28" s="28" t="s">
         <v>51</v>
@@ -7080,7 +7110,7 @@
         <v>55</v>
       </c>
       <c r="J28" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K28" s="28"/>
     </row>
@@ -7093,7 +7123,7 @@
         <v>437</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="E29" s="28" t="s">
         <v>51</v>
@@ -7111,7 +7141,7 @@
         <v>55</v>
       </c>
       <c r="J29" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K29" s="28"/>
     </row>
@@ -7124,7 +7154,7 @@
         <v>438</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="E30" s="28" t="s">
         <v>51</v>
@@ -7142,7 +7172,7 @@
         <v>55</v>
       </c>
       <c r="J30" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K30" s="28"/>
     </row>
@@ -7155,7 +7185,7 @@
         <v>439</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="E31" s="28" t="s">
         <v>51</v>
@@ -7173,7 +7203,7 @@
         <v>55</v>
       </c>
       <c r="J31" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K31" s="28"/>
     </row>
@@ -7183,10 +7213,10 @@
         <v>440</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="E32" s="28" t="s">
         <v>51</v>
@@ -7204,7 +7234,7 @@
         <v>55</v>
       </c>
       <c r="J32" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K32" s="28"/>
     </row>
@@ -7214,10 +7244,10 @@
         <v>441</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="E33" s="28" t="s">
         <v>51</v>
@@ -7235,7 +7265,7 @@
         <v>55</v>
       </c>
       <c r="J33" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K33" s="28"/>
     </row>
@@ -7245,10 +7275,10 @@
         <v>442</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="E34" s="28" t="s">
         <v>51</v>
@@ -7266,7 +7296,7 @@
         <v>55</v>
       </c>
       <c r="J34" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K34" s="28"/>
     </row>
@@ -7276,10 +7306,10 @@
         <v>443</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="E35" s="28" t="s">
         <v>51</v>
@@ -7297,7 +7327,7 @@
         <v>55</v>
       </c>
       <c r="J35" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K35" s="28"/>
     </row>
@@ -7307,10 +7337,10 @@
         <v>444</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="E36" s="28" t="s">
         <v>51</v>
@@ -7328,7 +7358,7 @@
         <v>55</v>
       </c>
       <c r="J36" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K36" s="28"/>
     </row>
@@ -7338,10 +7368,10 @@
         <v>445</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="E37" s="28" t="s">
         <v>51</v>
@@ -7359,7 +7389,7 @@
         <v>55</v>
       </c>
       <c r="J37" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K37" s="28"/>
     </row>
@@ -7369,10 +7399,10 @@
         <v>446</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="E38" s="28" t="s">
         <v>51</v>
@@ -7390,7 +7420,7 @@
         <v>55</v>
       </c>
       <c r="J38" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K38" s="28"/>
     </row>
@@ -7400,10 +7430,10 @@
         <v>447</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="E39" s="28" t="s">
         <v>51</v>
@@ -7421,7 +7451,7 @@
         <v>55</v>
       </c>
       <c r="J39" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K39" s="28"/>
     </row>
@@ -7431,10 +7461,10 @@
         <v>448</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="E40" s="28" t="s">
         <v>51</v>
@@ -7452,7 +7482,7 @@
         <v>55</v>
       </c>
       <c r="J40" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K40" s="28"/>
     </row>
@@ -7462,10 +7492,10 @@
         <v>449</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="E41" s="28" t="s">
         <v>51</v>
@@ -7483,7 +7513,7 @@
         <v>55</v>
       </c>
       <c r="J41" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K41" s="28"/>
     </row>
@@ -7493,10 +7523,10 @@
         <v>454</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="E42" s="28" t="s">
         <v>51</v>
@@ -7514,7 +7544,7 @@
         <v>55</v>
       </c>
       <c r="J42" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K42" s="28"/>
     </row>
@@ -7524,10 +7554,10 @@
         <v>457</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="E43" s="28" t="s">
         <v>51</v>
@@ -7545,7 +7575,7 @@
         <v>55</v>
       </c>
       <c r="J43" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K43" s="28"/>
     </row>
@@ -7555,10 +7585,10 @@
         <v>458</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="E44" s="28" t="s">
         <v>51</v>
@@ -7576,7 +7606,7 @@
         <v>55</v>
       </c>
       <c r="J44" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K44" s="28"/>
     </row>
@@ -7586,10 +7616,10 @@
         <v>459</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="E45" s="28" t="s">
         <v>51</v>
@@ -7607,7 +7637,7 @@
         <v>55</v>
       </c>
       <c r="J45" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K45" s="28"/>
     </row>
@@ -7617,10 +7647,10 @@
         <v>455</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="E46" s="28" t="s">
         <v>241</v>
@@ -7650,10 +7680,10 @@
         <v>460</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="E47" s="28" t="s">
         <v>51</v>
@@ -7671,7 +7701,7 @@
         <v>55</v>
       </c>
       <c r="J47" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K47" s="28"/>
     </row>
@@ -7681,10 +7711,10 @@
         <v>461</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="E48" s="28" t="s">
         <v>51</v>
@@ -7702,7 +7732,7 @@
         <v>55</v>
       </c>
       <c r="J48" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K48" s="28"/>
     </row>
@@ -7712,10 +7742,10 @@
         <v>462</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="E49" s="28" t="s">
         <v>51</v>
@@ -7733,7 +7763,7 @@
         <v>55</v>
       </c>
       <c r="J49" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K49" s="28"/>
     </row>
@@ -7743,10 +7773,10 @@
         <v>463</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D50" s="31" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>51</v>
@@ -7764,7 +7794,7 @@
         <v>55</v>
       </c>
       <c r="J50" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K50" s="28"/>
     </row>
@@ -7774,10 +7804,10 @@
         <v>464</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="E51" s="28" t="s">
         <v>51</v>
@@ -7795,7 +7825,7 @@
         <v>55</v>
       </c>
       <c r="J51" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K51" s="28"/>
     </row>
@@ -7805,10 +7835,10 @@
         <v>465</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="E52" s="28" t="s">
         <v>51</v>
@@ -7826,7 +7856,7 @@
         <v>55</v>
       </c>
       <c r="J52" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K52" s="28"/>
     </row>
@@ -7836,10 +7866,10 @@
         <v>456</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="E53" s="28" t="s">
         <v>241</v>
@@ -7869,10 +7899,10 @@
         <v>466</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>51</v>
@@ -7890,7 +7920,7 @@
         <v>55</v>
       </c>
       <c r="J54" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K54" s="28"/>
     </row>
@@ -7900,10 +7930,10 @@
         <v>467</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="E55" s="28" t="s">
         <v>51</v>
@@ -7921,7 +7951,7 @@
         <v>55</v>
       </c>
       <c r="J55" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K55" s="28"/>
     </row>
@@ -7931,10 +7961,10 @@
         <v>468</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="E56" s="28" t="s">
         <v>51</v>
@@ -7952,7 +7982,7 @@
         <v>55</v>
       </c>
       <c r="J56" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K56" s="28"/>
     </row>
@@ -7962,10 +7992,10 @@
         <v>469</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="E57" s="28" t="s">
         <v>51</v>
@@ -7983,7 +8013,7 @@
         <v>55</v>
       </c>
       <c r="J57" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K57" s="28"/>
     </row>
@@ -7993,10 +8023,10 @@
         <v>470</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E58" s="28" t="s">
         <v>51</v>
@@ -8014,7 +8044,7 @@
         <v>55</v>
       </c>
       <c r="J58" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K58" s="28"/>
     </row>
@@ -8024,10 +8054,10 @@
         <v>471</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D59" s="31" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="E59" s="28" t="s">
         <v>51</v>
@@ -8045,7 +8075,7 @@
         <v>55</v>
       </c>
       <c r="J59" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K59" s="28"/>
     </row>
@@ -8055,10 +8085,10 @@
         <v>477</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D60" s="31" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="E60" s="28" t="s">
         <v>241</v>
@@ -8088,10 +8118,10 @@
         <v>474</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="E61" s="28" t="s">
         <v>241</v>
@@ -8121,10 +8151,10 @@
         <v>472</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D62" s="31" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="E62" s="28" t="s">
         <v>51</v>
@@ -8142,7 +8172,7 @@
         <v>55</v>
       </c>
       <c r="J62" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K62" s="28"/>
     </row>
@@ -8152,10 +8182,10 @@
         <v>475</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D63" s="31" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="E63" s="28" t="s">
         <v>241</v>
@@ -8185,10 +8215,10 @@
         <v>478</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D64" s="31" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="E64" s="28" t="s">
         <v>51</v>
@@ -8206,7 +8236,7 @@
         <v>55</v>
       </c>
       <c r="J64" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K64" s="28"/>
     </row>
@@ -8216,28 +8246,28 @@
         <v>473</v>
       </c>
       <c r="C65" s="28" t="s">
+        <v>516</v>
+      </c>
+      <c r="D65" s="31" t="s">
+        <v>664</v>
+      </c>
+      <c r="E65" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="F65" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G65" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="H65" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="I65" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="J65" s="28" t="s">
         <v>517</v>
-      </c>
-      <c r="D65" s="31" t="s">
-        <v>668</v>
-      </c>
-      <c r="E65" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="F65" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="G65" s="28" t="s">
-        <v>218</v>
-      </c>
-      <c r="H65" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="I65" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="J65" s="28" t="s">
-        <v>518</v>
       </c>
       <c r="K65" s="28"/>
     </row>
@@ -8268,7 +8298,7 @@
         <v>55</v>
       </c>
       <c r="J66" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K66" s="28"/>
     </row>
@@ -8362,8 +8392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:K2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -8429,7 +8459,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -8443,10 +8473,10 @@
         <v>220</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>519</v>
+        <v>681</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>52</v>
@@ -8461,7 +8491,7 @@
         <v>55</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>232</v>
@@ -8475,7 +8505,7 @@
         <v>221</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>80</v>
@@ -8507,7 +8537,7 @@
         <v>33</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>32</v>
@@ -8536,7 +8566,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>34</v>
@@ -8583,7 +8613,7 @@
         <v>55</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -8594,7 +8624,7 @@
         <v>227</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>228</v>
@@ -8623,7 +8653,7 @@
         <v>230</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>231</v>
@@ -8655,7 +8685,7 @@
         <v>234</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>235</v>
@@ -8684,7 +8714,7 @@
         <v>240</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>241</v>
@@ -8716,7 +8746,7 @@
         <v>408</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>51</v>
@@ -8734,7 +8764,7 @@
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -8745,7 +8775,7 @@
         <v>479</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>34</v>
@@ -8774,7 +8804,7 @@
         <v>409</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>51</v>
@@ -8792,7 +8822,7 @@
         <v>55</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -8803,7 +8833,7 @@
         <v>480</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>34</v>
@@ -8832,7 +8862,7 @@
         <v>410</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>51</v>
@@ -8850,7 +8880,7 @@
         <v>55</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
@@ -8861,7 +8891,7 @@
         <v>411</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>51</v>
@@ -8879,7 +8909,7 @@
         <v>55</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
@@ -8890,7 +8920,7 @@
         <v>412</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>51</v>
@@ -8908,7 +8938,7 @@
         <v>55</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
@@ -8919,7 +8949,7 @@
         <v>413</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>51</v>
@@ -8937,7 +8967,7 @@
         <v>55</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
@@ -8948,7 +8978,7 @@
         <v>414</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>51</v>
@@ -8966,7 +8996,7 @@
         <v>55</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
@@ -8977,7 +9007,7 @@
         <v>481</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>34</v>
@@ -9006,7 +9036,7 @@
         <v>451</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>51</v>
@@ -9024,7 +9054,7 @@
         <v>55</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
@@ -9035,7 +9065,7 @@
         <v>482</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>34</v>
@@ -9064,7 +9094,7 @@
         <v>453</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>51</v>
@@ -9082,7 +9112,7 @@
         <v>55</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
@@ -9093,7 +9123,7 @@
         <v>415</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>51</v>
@@ -9111,7 +9141,7 @@
         <v>55</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
@@ -9122,7 +9152,7 @@
         <v>416</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>51</v>
@@ -9140,7 +9170,7 @@
         <v>55</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
@@ -9151,7 +9181,7 @@
         <v>431</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>51</v>
@@ -9169,7 +9199,7 @@
         <v>55</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
@@ -9180,7 +9210,7 @@
         <v>436</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>51</v>
@@ -9198,7 +9228,7 @@
         <v>55</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
@@ -9209,7 +9239,7 @@
         <v>437</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>51</v>
@@ -9227,7 +9257,7 @@
         <v>55</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
@@ -9238,7 +9268,7 @@
         <v>438</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>51</v>
@@ -9256,7 +9286,7 @@
         <v>55</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
@@ -9267,7 +9297,7 @@
         <v>439</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>51</v>
@@ -9285,7 +9315,7 @@
         <v>55</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.2">
@@ -9293,10 +9323,10 @@
         <v>440</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>51</v>
@@ -9314,7 +9344,7 @@
         <v>55</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
@@ -9322,10 +9352,10 @@
         <v>441</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>51</v>
@@ -9343,7 +9373,7 @@
         <v>55</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
@@ -9351,10 +9381,10 @@
         <v>442</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>51</v>
@@ -9372,7 +9402,7 @@
         <v>55</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
@@ -9380,10 +9410,10 @@
         <v>443</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>51</v>
@@ -9401,7 +9431,7 @@
         <v>55</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
@@ -9409,10 +9439,10 @@
         <v>444</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>51</v>
@@ -9430,7 +9460,7 @@
         <v>55</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
@@ -9438,10 +9468,10 @@
         <v>445</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>51</v>
@@ -9459,7 +9489,7 @@
         <v>55</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
@@ -9467,10 +9497,10 @@
         <v>446</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>51</v>
@@ -9488,7 +9518,7 @@
         <v>55</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
@@ -9496,10 +9526,10 @@
         <v>447</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>51</v>
@@ -9517,7 +9547,7 @@
         <v>55</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -9525,10 +9555,10 @@
         <v>448</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>51</v>
@@ -9546,7 +9576,7 @@
         <v>55</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
@@ -9554,10 +9584,10 @@
         <v>449</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>51</v>
@@ -9575,7 +9605,7 @@
         <v>55</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
@@ -9583,10 +9613,10 @@
         <v>454</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>51</v>
@@ -9604,7 +9634,7 @@
         <v>55</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
@@ -9612,10 +9642,10 @@
         <v>457</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>51</v>
@@ -9633,7 +9663,7 @@
         <v>55</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
@@ -9641,10 +9671,10 @@
         <v>458</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>51</v>
@@ -9662,7 +9692,7 @@
         <v>55</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
@@ -9670,10 +9700,10 @@
         <v>459</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>51</v>
@@ -9691,7 +9721,7 @@
         <v>55</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
@@ -9699,10 +9729,10 @@
         <v>455</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>241</v>
@@ -9731,10 +9761,10 @@
         <v>460</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>51</v>
@@ -9752,7 +9782,7 @@
         <v>55</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
@@ -9760,10 +9790,10 @@
         <v>461</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>51</v>
@@ -9781,7 +9811,7 @@
         <v>55</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.2">
@@ -9789,10 +9819,10 @@
         <v>462</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>51</v>
@@ -9810,7 +9840,7 @@
         <v>55</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.2">
@@ -9818,10 +9848,10 @@
         <v>463</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>51</v>
@@ -9839,7 +9869,7 @@
         <v>55</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
@@ -9847,10 +9877,10 @@
         <v>464</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>51</v>
@@ -9868,7 +9898,7 @@
         <v>55</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.2">
@@ -9876,10 +9906,10 @@
         <v>465</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>51</v>
@@ -9897,7 +9927,7 @@
         <v>55</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.2">
@@ -9905,10 +9935,10 @@
         <v>456</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>241</v>
@@ -9937,10 +9967,10 @@
         <v>466</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D54" s="24" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>51</v>
@@ -9958,7 +9988,7 @@
         <v>55</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.2">
@@ -9966,10 +9996,10 @@
         <v>467</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D55" s="24" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>51</v>
@@ -9987,7 +10017,7 @@
         <v>55</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.2">
@@ -9995,10 +10025,10 @@
         <v>468</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>51</v>
@@ -10016,7 +10046,7 @@
         <v>55</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.2">
@@ -10024,10 +10054,10 @@
         <v>469</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>51</v>
@@ -10045,7 +10075,7 @@
         <v>55</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.2">
@@ -10053,10 +10083,10 @@
         <v>470</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D58" s="24" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>51</v>
@@ -10074,7 +10104,7 @@
         <v>55</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.2">
@@ -10082,10 +10112,10 @@
         <v>471</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>51</v>
@@ -10103,7 +10133,7 @@
         <v>55</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.2">
@@ -10111,10 +10141,10 @@
         <v>477</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D60" s="24" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>241</v>
@@ -10143,10 +10173,10 @@
         <v>474</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D61" s="24" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>241</v>
@@ -10175,10 +10205,10 @@
         <v>472</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D62" s="24" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>51</v>
@@ -10196,7 +10226,7 @@
         <v>55</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.2">
@@ -10204,10 +10234,10 @@
         <v>475</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D63" s="24" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>241</v>
@@ -10236,10 +10266,10 @@
         <v>478</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D64" s="24" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>51</v>
@@ -10257,7 +10287,7 @@
         <v>55</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.2">
@@ -10265,28 +10295,28 @@
         <v>473</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D65" s="24" t="s">
+        <v>578</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J65" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="D65" s="24" t="s">
-        <v>580</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J65" s="1" t="s">
-        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -10366,8 +10396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03FDA06-9F92-49C6-8A00-2EE1AEC24A99}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10413,16 +10443,16 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="C2" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -10444,9 +10474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F2B47B-56D5-4D18-829C-61064082089E}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10454,6 +10482,7 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -10472,41 +10501,41 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="C2" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="D2" s="27" t="str">
         <f>E2</f>
         <v>Rudra_2806</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="C3" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C4" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="D4" s="6" t="str">
         <f>emailCred!A2</f>
-        <v>Spidey@1990</v>
+        <v>Thanos@1990</v>
       </c>
     </row>
   </sheetData>
@@ -10520,7 +10549,7 @@
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10618,50 +10647,137 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AMK3"/>
+  <dimension ref="A1:AMK9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="102.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="1025" width="8.42578125" collapsed="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="56.7109375" style="34" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="38.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="1025" width="8.42578125" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>483</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="E1" t="s">
+        <v>679</v>
+      </c>
+      <c r="F1" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="str">
+        <f>A3</f>
+        <v>Thanos@1990</v>
+      </c>
+      <c r="B2" s="34" t="str">
+        <f>E2</f>
+        <v>shailendra.rajawat@nextgenclearing.com</v>
+      </c>
+      <c r="C2" s="34" t="str">
+        <f>E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5</f>
+        <v>shailendra.rajawat@nextgenclearing.com,prafull.barve@nextgenclearing.com,ivana.jandrecic@nextgenclearing.com,dario.curjak@nextgenclearing.com</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>682</v>
+      </c>
+      <c r="C3" s="34" t="str">
+        <f>E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E6&amp;","&amp;E7</f>
+        <v>shailendra.rajawat@nextgenclearing.com,prafull.barve@nextgenclearing.com,ivana.jandrecic@nextgenclearing.com,aarjav.thakore@nextgenclearing.com,micky.priya@nextgenclearing.com</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="5"/>
+      <c r="F3" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="5" t="s">
+        <v>671</v>
+      </c>
+      <c r="F4" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>672</v>
+      </c>
+      <c r="F5" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="F6" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="5" t="s">
+        <v>674</v>
+      </c>
+      <c r="F7" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F8" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="5" t="s">
+        <v>676</v>
+      </c>
+      <c r="F9" t="s">
+        <v>678</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="Thanos@1990" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" display="shailendra.rajawat@nextgenclearing.com" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{E79489D9-2090-40A0-A045-D537065B7547}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{151A16B0-D4CF-4060-9FC2-B663C0C66EB9}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{B8DAAD96-1BED-45B8-AC9F-50A507FB7460}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{AED63D9F-CCE4-44C9-B17C-D6C2E46BE679}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{A7DA2543-1C8C-4B75-A1B0-F70E000F582F}"/>
+    <hyperlink ref="E7" r:id="rId8" xr:uid="{5A109B21-233F-4CDD-AFEB-688FECD0D94C}"/>
+    <hyperlink ref="E8" r:id="rId9" xr:uid="{60AF829D-781E-468D-9683-86836D64173A}"/>
+    <hyperlink ref="E9" r:id="rId10" xr:uid="{DAA6F6D8-EBEF-48D7-8C04-51636A966F9E}"/>
+    <hyperlink ref="A3" r:id="rId11" xr:uid="{845AE483-01AA-413A-85B9-23469542E415}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>